<commit_message>
add spreadsheet search functions. add finding user name func to check_pw()
</commit_message>
<xml_diff>
--- a/work_log.xlsx
+++ b/work_log.xlsx
@@ -5,23 +5,47 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="22488" windowHeight="9024" activeTab="1"/>
+    <workbookView windowWidth="22488" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="workers" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="1" r:id="rId2"/>
+    <sheet name=" 張三" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>2348</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>3445</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>4868</t>
+  </si>
+  <si>
+    <t>Sammy</t>
+  </si>
+  <si>
+    <t>2476</t>
+  </si>
+  <si>
+    <t>Jessica</t>
   </si>
   <si>
     <t>check out time</t>
@@ -44,13 +68,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +83,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -75,8 +114,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -106,6 +199,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -113,20 +214,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -134,79 +221,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -219,12 +236,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -237,90 +272,126 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -333,73 +404,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,6 +427,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -424,30 +465,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -476,17 +493,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -504,163 +510,175 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,20 +1025,55 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="8.88888888888889" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1034,8 +1087,8 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1049,21 +1102,21 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>44060.6240393519</v>

</xml_diff>

<commit_message>
homeworks: 1) finding the error of writing log. 2)check the log is all correct.
</commit_message>
<xml_diff>
--- a/work_log.xlsx
+++ b/work_log.xlsx
@@ -69,11 +69,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -92,12 +92,89 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -105,6 +182,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -112,66 +198,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -183,46 +221,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,37 +237,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,145 +417,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,21 +436,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,7 +474,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,15 +496,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -528,18 +504,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -549,137 +549,137 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="2">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="35" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1091,7 +1091,7 @@
   <sheetPr/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="E2" s="1">
         <f t="shared" ref="E2:E13" si="0">(D2-C2)*24</f>
-        <v>1.99999995151302</v>
+        <v>1.9999999513384</v>
       </c>
     </row>
     <row r="3" spans="1:5">

</xml_diff>